<commit_message>
Create download excel function and root
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_virements_xlsx/état_des_virements_3_2022.xlsx
+++ b/download/generated situation/état_des_virements_xlsx/état_des_virements_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,252 +417,39 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Anas test</v>
+        <v>Yassine test</v>
       </c>
       <c r="B2" t="str">
-        <v>25689432</v>
+        <v>123</v>
       </c>
       <c r="C2" t="str">
-        <v>116978532135755179843543</v>
+        <v>112354646135431354351432</v>
       </c>
       <c r="D2" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E2" t="str">
-        <v>32135</v>
+        <v>13213</v>
       </c>
       <c r="F2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="G2" t="str">
-        <v>001/DR 1</v>
+        <v>001/test DR</v>
       </c>
       <c r="H2" t="str">
         <v>mensuelle</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="K2">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B3" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C3" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E3" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G3" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B4" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C4" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E4" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G4" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B5" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C5" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D5" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E5" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G5" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B6" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C6" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D6" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E6" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G6" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B7" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C7" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D7" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E7" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G7" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Anas test</v>
-      </c>
-      <c r="B8" t="str">
-        <v>25689432</v>
-      </c>
-      <c r="C8" t="str">
-        <v>116978532135755179843543</v>
-      </c>
-      <c r="D8" t="str">
-        <v>1354</v>
-      </c>
-      <c r="E8" t="str">
-        <v>32135</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G8" t="str">
-        <v>001/DR 1</v>
-      </c>
-      <c r="H8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>33750</v>
+        <v>42500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>